<commit_message>
Updates for Out There 2
</commit_message>
<xml_diff>
--- a/jsf_fleet_habs.xlsx
+++ b/jsf_fleet_habs.xlsx
@@ -1,36 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26929"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dare/Documents/personal/posthuman/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0144BBAB-BA03-1E4A-A524-86736BCA53B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Fleet structure" sheetId="1" r:id="rId1"/>
     <sheet name="Hab populations" sheetId="2" r:id="rId2"/>
     <sheet name="Ship stats" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="400">
   <si>
     <t>JSF: Structure</t>
   </si>
@@ -1209,13 +1203,34 @@
   </si>
   <si>
     <t>Beehive + Torus</t>
+  </si>
+  <si>
+    <t>Havana de Cielo</t>
+  </si>
+  <si>
+    <t>Wannabe</t>
+  </si>
+  <si>
+    <t>Sport Team</t>
+  </si>
+  <si>
+    <t>Wolverines</t>
+  </si>
+  <si>
+    <t>Draker</t>
+  </si>
+  <si>
+    <t>Relampago</t>
+  </si>
+  <si>
+    <t>Pierre Sumbon (D)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1238,6 +1253,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1256,8 +1287,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1269,7 +1302,9 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1540,14 +1575,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1555,7 +1590,7 @@
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="34.5" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" customWidth="1"/>
@@ -1566,12 +1601,12 @@
     <col min="7" max="7" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1594,7 +1629,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1611,7 +1646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="B4" t="s">
         <v>54</v>
       </c>
@@ -1628,7 +1663,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="C5" t="s">
         <v>13</v>
       </c>
@@ -1642,7 +1677,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="B6" t="s">
         <v>294</v>
       </c>
@@ -1659,7 +1694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -1673,7 +1708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="C8" t="s">
         <v>21</v>
       </c>
@@ -1687,7 +1722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1710,7 +1745,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="B10" t="s">
         <v>27</v>
       </c>
@@ -1724,7 +1759,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="B11" t="s">
         <v>30</v>
       </c>
@@ -1741,7 +1776,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="C12" t="s">
         <v>303</v>
       </c>
@@ -1755,7 +1790,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="C13" t="s">
         <v>343</v>
       </c>
@@ -1769,7 +1804,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="C14" t="s">
         <v>341</v>
       </c>
@@ -1783,7 +1818,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="C15" t="s">
         <v>345</v>
       </c>
@@ -1797,7 +1832,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="C16" t="s">
         <v>346</v>
       </c>
@@ -1811,7 +1846,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="C17" t="s">
         <v>347</v>
       </c>
@@ -1825,7 +1860,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="C18" t="s">
         <v>348</v>
       </c>
@@ -1839,7 +1874,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="C19" t="s">
         <v>349</v>
       </c>
@@ -1853,7 +1888,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="C20" t="s">
         <v>350</v>
       </c>
@@ -1867,7 +1902,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1887,7 +1922,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="C22" t="s">
         <v>50</v>
       </c>
@@ -1901,7 +1936,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="B23" t="s">
         <v>36</v>
       </c>
@@ -1918,7 +1953,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="C24" t="s">
         <v>38</v>
       </c>
@@ -1932,7 +1967,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="C25" t="s">
         <v>40</v>
       </c>
@@ -1946,7 +1981,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="C26" t="s">
         <v>42</v>
       </c>
@@ -1960,7 +1995,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="C27" t="s">
         <v>43</v>
       </c>
@@ -1974,7 +2009,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="C28" t="s">
         <v>45</v>
       </c>
@@ -1988,7 +2023,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="C29" t="s">
         <v>47</v>
       </c>
@@ -2002,7 +2037,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="B30" t="s">
         <v>53</v>
       </c>
@@ -2016,7 +2051,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="C31" t="s">
         <v>324</v>
       </c>
@@ -2030,7 +2065,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="C32" t="s">
         <v>146</v>
       </c>
@@ -2044,7 +2079,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="B33" t="s">
         <v>57</v>
       </c>
@@ -2061,7 +2096,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="C34" t="s">
         <v>60</v>
       </c>
@@ -2075,7 +2110,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="B35" t="s">
         <v>281</v>
       </c>
@@ -2095,7 +2130,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="B36" t="s">
         <v>289</v>
       </c>
@@ -2115,7 +2150,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>62</v>
       </c>
@@ -2135,7 +2170,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="B38" t="s">
         <v>65</v>
       </c>
@@ -2152,7 +2187,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="B39" t="s">
         <v>68</v>
       </c>
@@ -2169,7 +2204,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="B40" t="s">
         <v>71</v>
       </c>
@@ -2186,7 +2221,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="B41" t="s">
         <v>74</v>
       </c>
@@ -2203,7 +2238,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="C42" t="s">
         <v>305</v>
       </c>
@@ -2214,7 +2249,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -2234,7 +2269,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="B44" t="s">
         <v>80</v>
       </c>
@@ -2248,7 +2283,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="B45" t="s">
         <v>84</v>
       </c>
@@ -2262,7 +2297,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>87</v>
       </c>
@@ -2282,7 +2317,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="B47" t="s">
         <v>90</v>
       </c>
@@ -2296,7 +2331,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="B48" t="s">
         <v>94</v>
       </c>
@@ -2313,7 +2348,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="B49" t="s">
         <v>98</v>
       </c>
@@ -2321,7 +2356,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>99</v>
       </c>
@@ -2341,7 +2376,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="C51" t="s">
         <v>101</v>
       </c>
@@ -2355,7 +2390,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="B52" t="s">
         <v>103</v>
       </c>
@@ -2375,7 +2410,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="C53" t="s">
         <v>105</v>
       </c>
@@ -2392,7 +2427,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="C54" t="s">
         <v>108</v>
       </c>
@@ -2409,7 +2444,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="C55" t="s">
         <v>110</v>
       </c>
@@ -2426,7 +2461,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="C56" t="s">
         <v>286</v>
       </c>
@@ -2443,7 +2478,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="B57" t="s">
         <v>112</v>
       </c>
@@ -2460,7 +2495,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="C58" t="s">
         <v>115</v>
       </c>
@@ -2474,7 +2509,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="C59" t="s">
         <v>117</v>
       </c>
@@ -2488,7 +2523,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="C60" t="s">
         <v>119</v>
       </c>
@@ -2502,7 +2537,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="B61" t="s">
         <v>121</v>
       </c>
@@ -2519,7 +2554,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="C62" t="s">
         <v>295</v>
       </c>
@@ -2533,7 +2568,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="C63" t="s">
         <v>299</v>
       </c>
@@ -2547,7 +2582,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="C64" t="s">
         <v>335</v>
       </c>
@@ -2561,7 +2596,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8">
       <c r="C65" s="4" t="s">
         <v>326</v>
       </c>
@@ -2578,7 +2613,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8">
       <c r="C66" t="s">
         <v>297</v>
       </c>
@@ -2592,7 +2627,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8">
       <c r="C67" t="s">
         <v>124</v>
       </c>
@@ -2609,7 +2644,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8">
       <c r="B68" t="s">
         <v>125</v>
       </c>
@@ -2617,7 +2652,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8">
       <c r="B69" t="s">
         <v>127</v>
       </c>
@@ -2631,7 +2666,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8">
       <c r="B70" t="s">
         <v>130</v>
       </c>
@@ -2645,7 +2680,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>134</v>
       </c>
@@ -2669,7 +2704,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8">
       <c r="B72" t="s">
         <v>136</v>
       </c>
@@ -2683,7 +2718,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8">
       <c r="C73" t="s">
         <v>337</v>
       </c>
@@ -2697,7 +2732,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8">
       <c r="C74" t="s">
         <v>338</v>
       </c>
@@ -2711,7 +2746,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8">
       <c r="C75" t="s">
         <v>137</v>
       </c>
@@ -2725,7 +2760,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8">
       <c r="B76" t="s">
         <v>139</v>
       </c>
@@ -2742,7 +2777,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8">
       <c r="C77" t="s">
         <v>320</v>
       </c>
@@ -2753,7 +2788,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8">
       <c r="C78" t="s">
         <v>270</v>
       </c>
@@ -2767,7 +2802,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8">
       <c r="C79" t="s">
         <v>272</v>
       </c>
@@ -2781,7 +2816,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8">
       <c r="C80" t="s">
         <v>273</v>
       </c>
@@ -2795,7 +2830,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8">
       <c r="C81" s="4" t="s">
         <v>328</v>
       </c>
@@ -2812,7 +2847,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8">
       <c r="B82" t="s">
         <v>141</v>
       </c>
@@ -2829,7 +2864,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8">
       <c r="B83" t="s">
         <v>291</v>
       </c>
@@ -2846,7 +2881,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8">
       <c r="B84" t="s">
         <v>307</v>
       </c>
@@ -2863,7 +2898,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8">
       <c r="C85" t="s">
         <v>323</v>
       </c>
@@ -2877,7 +2912,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8">
       <c r="C86" t="s">
         <v>330</v>
       </c>
@@ -2891,7 +2926,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8">
       <c r="B87" t="s">
         <v>314</v>
       </c>
@@ -2908,7 +2943,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>144</v>
       </c>
@@ -2924,19 +2959,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="17.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.1640625" customWidth="1"/>
@@ -2948,7 +2988,7 @@
     <col min="13" max="13" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>175</v>
       </c>
@@ -2976,8 +3016,11 @@
       <c r="I1" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>180</v>
       </c>
@@ -2997,7 +3040,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -3014,7 +3057,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>224</v>
       </c>
@@ -3037,7 +3080,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>258</v>
       </c>
@@ -3058,10 +3101,10 @@
       </c>
       <c r="K5" s="3">
         <f>SUM(G1:G123)</f>
-        <v>23550500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>23560500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>187</v>
       </c>
@@ -3081,7 +3124,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>187</v>
       </c>
@@ -3101,7 +3144,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>187</v>
       </c>
@@ -3121,7 +3164,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>187</v>
       </c>
@@ -3137,8 +3180,11 @@
       <c r="G9" s="3">
         <v>200000</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>187</v>
       </c>
@@ -3154,8 +3200,11 @@
       <c r="G10" s="3">
         <v>100000</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1">
       <c r="A11" t="s">
         <v>187</v>
       </c>
@@ -3166,7 +3215,9 @@
       <c r="D11" t="s">
         <v>366</v>
       </c>
-      <c r="E11"/>
+      <c r="E11" t="s">
+        <v>399</v>
+      </c>
       <c r="F11" t="s">
         <v>189</v>
       </c>
@@ -3176,7 +3227,7 @@
       <c r="H11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>187</v>
       </c>
@@ -3193,7 +3244,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>228</v>
       </c>
@@ -3213,7 +3264,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>222</v>
       </c>
@@ -3233,7 +3284,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>203</v>
       </c>
@@ -3250,7 +3301,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>185</v>
       </c>
@@ -3273,7 +3324,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>185</v>
       </c>
@@ -3290,7 +3341,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>185</v>
       </c>
@@ -3313,7 +3364,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>185</v>
       </c>
@@ -3328,6 +3379,9 @@
       </c>
       <c r="G19" s="3">
         <v>1200000</v>
+      </c>
+      <c r="J19" t="s">
+        <v>396</v>
       </c>
       <c r="L19" t="s">
         <v>388</v>
@@ -3337,7 +3391,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>185</v>
       </c>
@@ -3361,7 +3415,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>185</v>
       </c>
@@ -3385,7 +3439,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>185</v>
       </c>
@@ -3409,7 +3463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>185</v>
       </c>
@@ -3429,7 +3483,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -3449,7 +3503,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>211</v>
       </c>
@@ -3473,7 +3527,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>211</v>
       </c>
@@ -3490,7 +3544,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>211</v>
       </c>
@@ -3507,7 +3561,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>193</v>
       </c>
@@ -3524,7 +3578,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>219</v>
       </c>
@@ -3544,7 +3598,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>197</v>
       </c>
@@ -3570,7 +3624,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>174</v>
       </c>
@@ -3590,7 +3644,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>261</v>
       </c>
@@ -3610,7 +3664,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
         <v>215</v>
       </c>
@@ -3630,7 +3684,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
         <v>183</v>
       </c>
@@ -3653,7 +3707,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="B35" t="s">
         <v>309</v>
       </c>
@@ -3673,7 +3727,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="B36" t="s">
         <v>199</v>
       </c>
@@ -3690,7 +3744,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="B37" t="s">
         <v>311</v>
       </c>
@@ -3710,7 +3764,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="B38" t="s">
         <v>202</v>
       </c>
@@ -3724,7 +3778,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="B39" t="s">
         <v>205</v>
       </c>
@@ -3736,6 +3790,23 @@
       </c>
       <c r="G39" s="3">
         <v>900</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="B40" t="s">
+        <v>393</v>
+      </c>
+      <c r="C40" t="s">
+        <v>394</v>
+      </c>
+      <c r="F40" t="s">
+        <v>182</v>
+      </c>
+      <c r="G40" s="3">
+        <v>10000</v>
+      </c>
+      <c r="H40" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3744,11 +3815,17 @@
     <sortCondition descending="1" ref="G2:G39"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3756,7 +3833,7 @@
       <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="3" max="4" width="8.33203125" customWidth="1"/>
@@ -3765,7 +3842,7 @@
     <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>229</v>
       </c>
@@ -3809,7 +3886,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>149</v>
       </c>
@@ -3856,7 +3933,7 @@
         <v>264.49872231552229</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3894,7 +3971,7 @@
         <v>59.062085149273109</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4" t="s">
         <v>279</v>
       </c>
@@ -3940,5 +4017,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>